<commit_message>
Added DRA Landing Page script
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/DRA.xlsx
+++ b/src/test/resources/xls/DRA.xlsx
@@ -37,10 +37,10 @@
     <t>Y</t>
   </si>
   <si>
-    <t>Verify that, accessing of the URL  takes the user to DRA application Landing page</t>
-  </si>
-  <si>
     <t>OBT</t>
+  </si>
+  <si>
+    <t>Verify that, accessing of the URL  takes the user to DRA application Landing page || Verify that DRA Landing page, displays application branding and logo || Verify that DRA Landing page, contains feature promotion and iconography in the marketing section || Verify that DRA Landing page, displays link to privacy statement and terms of use. || verify that DRA Landing page, displays the message and email id on the DRA landing page "Having trouble with sign-in? please contact DRA_support@thomsonreuters.com "</t>
   </si>
 </sst>
 </file>
@@ -411,7 +411,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -440,15 +440,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>8</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>7</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
Added New DRA Scripts
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/DRA.xlsx
+++ b/src/test/resources/xls/DRA.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="15">
   <si>
     <t>TCID</t>
   </si>
@@ -41,13 +41,56 @@
   </si>
   <si>
     <t>Verify that, accessing of the URL  takes the user to DRA application Landing page || Verify that DRA Landing page, displays application branding and logo || Verify that DRA Landing page, contains feature promotion and iconography in the marketing section || Verify that DRA Landing page, displays link to privacy statement and terms of use. || verify that DRA Landing page, displays the message and email id on the DRA landing page "Having trouble with sign-in? please contact DRA_support@thomsonreuters.com "</t>
+  </si>
+  <si>
+    <t>DRA002</t>
+  </si>
+  <si>
+    <t>DRA003</t>
+  </si>
+  <si>
+    <t>DRA004</t>
+  </si>
+  <si>
+    <t>Verify that user can skip the linking by clicking on "Not now button" on the modal "Already have an account? .. || Verify that once the user skips linking then user will not be prompted to link again.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Verify that user should be prompted to link accounts, when sign in first time on </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color indexed="8"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>DRA landing screen</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> using STeAM. (Note:User should already been sign into social)</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve"> Verify that when linking a social with a matching email, if the user click [X] cross mark on the screen then he will be taken back to the DRA Login page. || Verify that text on the modal "Already have an account? ..
+You have previously signed in with &lt;email address&gt; using LinkedIn
+To Protect your security, please sign into LinkedIn so that we can link your account.
+&lt;not now&gt; &lt;Sign in using Facebook&gt;" , when linking LinkedIn with steam ||Verify that when linking a social with a matching email, if the user clicks outside the Linking modal on the screen then nothing should happens</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -55,8 +98,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -66,6 +116,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -97,12 +153,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -408,10 +467,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -455,6 +514,51 @@
       </c>
       <c r="E2" s="2"/>
     </row>
+    <row r="3" spans="1:5" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="2"/>
+    </row>
+    <row r="4" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="2"/>
+    </row>
+    <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="2"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
DRA new script implementation
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/DRA.xlsx
+++ b/src/test/resources/xls/DRA.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="2640" windowWidth="13290" windowHeight="3840"/>
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="125725" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="27">
   <si>
     <t>TCID</t>
   </si>
@@ -112,12 +112,21 @@
   <si>
     <t>forgot PWD</t>
   </si>
+  <si>
+    <t>DRA5</t>
+  </si>
+  <si>
+    <t>Verify that ProfileFlyout links</t>
+  </si>
+  <si>
+    <t>OPQA-TBD</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -314,7 +323,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -349,7 +357,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -525,14 +532,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="14.42578125" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="34.42578125" customWidth="1" collapsed="1"/>
@@ -541,7 +548,7 @@
     <col min="5" max="5" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -558,7 +565,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="90">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
@@ -573,7 +580,7 @@
       </c>
       <c r="E2" s="2"/>
     </row>
-    <row r="3" spans="1:5" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="34.5" customHeight="1">
       <c r="A3" s="3" t="s">
         <v>9</v>
       </c>
@@ -588,7 +595,7 @@
       </c>
       <c r="E3" s="2"/>
     </row>
-    <row r="4" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="120">
       <c r="A4" s="3" t="s">
         <v>10</v>
       </c>
@@ -603,7 +610,7 @@
       </c>
       <c r="E4" s="2"/>
     </row>
-    <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="45">
       <c r="A5" s="3" t="s">
         <v>11</v>
       </c>
@@ -618,7 +625,7 @@
       </c>
       <c r="E5" s="2"/>
     </row>
-    <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="45">
       <c r="A6" s="5" t="s">
         <v>15</v>
       </c>
@@ -628,10 +635,12 @@
       <c r="C6" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="5"/>
+      <c r="D6" s="5" t="s">
+        <v>6</v>
+      </c>
       <c r="E6" s="5"/>
     </row>
-    <row r="7" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="45">
       <c r="A7" s="5" t="s">
         <v>18</v>
       </c>
@@ -641,10 +650,12 @@
       <c r="C7" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="6"/>
+      <c r="D7" s="6" t="s">
+        <v>6</v>
+      </c>
       <c r="E7" s="5"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5">
       <c r="A8" s="5" t="s">
         <v>19</v>
       </c>
@@ -654,10 +665,12 @@
       <c r="C8" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D8" s="5"/>
+      <c r="D8" s="5" t="s">
+        <v>6</v>
+      </c>
       <c r="E8" s="5"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5">
       <c r="A9" s="5" t="s">
         <v>21</v>
       </c>
@@ -667,8 +680,25 @@
       <c r="C9" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D9" s="5"/>
+      <c r="D9" s="5" t="s">
+        <v>6</v>
+      </c>
       <c r="E9" s="5"/>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E10" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Fixed DRA0010 and DRA0011 scripts
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/DRA.xlsx
+++ b/src/test/resources/xls/DRA.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="2640" windowWidth="13290" windowHeight="3840"/>
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725" concurrentCalc="0"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="29">
   <si>
     <t>TCID</t>
   </si>
@@ -92,9 +92,6 @@
     <t>OPQA-1688</t>
   </si>
   <si>
-    <t>Verify that user should  not be allowed to sign-in to DRA when email/password combination is incorrect and error message "Invalid Email/Password. Please try again." should be dispalyed as per  DRA Access - conditional text and error message document.</t>
-  </si>
-  <si>
     <t>DRA0011</t>
   </si>
   <si>
@@ -120,13 +117,23 @@
   </si>
   <si>
     <t>OPQA-TBD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify that user should  not be allowed to sign-in to DRA when email/password combination is incorrect and error message "Invalid Email/Password. Please try again." should be dispalyed as per  DRA Access - conditional text and error message document.
+</t>
+  </si>
+  <si>
+    <t>OPQA-4185 ||OPQA-4196</t>
+  </si>
+  <si>
+    <t>Verify that user should not be allowed to access DRA if the STeAM account is not tied to an active subscription with the "DRA_TARGET_DRUG" entitlement (SKU).|| Verify that Error message is displayed to the user, when DRA user who attempts to access DRA without an active DRA entitlement (STeAM SKU)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -323,6 +330,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -357,6 +365,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -532,14 +541,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.42578125" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="34.42578125" customWidth="1" collapsed="1"/>
@@ -548,7 +557,7 @@
     <col min="5" max="5" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -565,7 +574,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="90">
+    <row r="2" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
@@ -580,7 +589,7 @@
       </c>
       <c r="E2" s="2"/>
     </row>
-    <row r="3" spans="1:5" ht="34.5" customHeight="1">
+    <row r="3" spans="1:5" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>9</v>
       </c>
@@ -595,7 +604,7 @@
       </c>
       <c r="E3" s="2"/>
     </row>
-    <row r="4" spans="1:5" ht="120">
+    <row r="4" spans="1:5" ht="120" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>10</v>
       </c>
@@ -610,7 +619,7 @@
       </c>
       <c r="E4" s="2"/>
     </row>
-    <row r="5" spans="1:5" ht="45">
+    <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>11</v>
       </c>
@@ -625,7 +634,7 @@
       </c>
       <c r="E5" s="2"/>
     </row>
-    <row r="6" spans="1:5" ht="45">
+    <row r="6" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>15</v>
       </c>
@@ -633,67 +642,67 @@
         <v>16</v>
       </c>
       <c r="C6" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" s="5"/>
+    </row>
+    <row r="7" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E6" s="5"/>
-    </row>
-    <row r="7" spans="1:5" ht="45">
-      <c r="A7" s="5" t="s">
+      <c r="B7" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" s="5"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
         <v>18</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="E7" s="5"/>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="5" t="s">
-        <v>19</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>16</v>
       </c>
       <c r="C8" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" s="5"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D8" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E8" s="5"/>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" s="5" t="s">
+      <c r="B9" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="C9" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="D9" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" s="5"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D9" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E9" s="5"/>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" s="5" t="s">
+      <c r="B10" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="5" t="s">
         <v>24</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>25</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
Added Jira Id's to the testcases in DRA.xlsx
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/DRA.xlsx
+++ b/src/test/resources/xls/DRA.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="31">
   <si>
     <t>TCID</t>
   </si>
@@ -35,12 +35,6 @@
   </si>
   <si>
     <t>Y</t>
-  </si>
-  <si>
-    <t>OBT</t>
-  </si>
-  <si>
-    <t>Verify that, accessing of the URL  takes the user to DRA application Landing page || Verify that DRA Landing page, displays application branding and logo || Verify that DRA Landing page, contains feature promotion and iconography in the marketing section || Verify that DRA Landing page, displays link to privacy statement and terms of use. || verify that DRA Landing page, displays the message and email id on the DRA landing page "Having trouble with sign-in? please contact DRA_support@thomsonreuters.com "</t>
   </si>
   <si>
     <t>DRA002</t>
@@ -80,18 +74,9 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve"> Verify that when linking a social with a matching email, if the user click [X] cross mark on the screen then he will be taken back to the DRA Login page. || Verify that text on the modal "Already have an account? ..
-You have previously signed in with &lt;email address&gt; using LinkedIn
-To Protect your security, please sign into LinkedIn so that we can link your account.
-&lt;not now&gt; &lt;Sign in using Facebook&gt;" , when linking LinkedIn with steam ||Verify that when linking a social with a matching email, if the user clicks outside the Linking modal on the screen then nothing should happens</t>
-  </si>
-  <si>
     <t>DRA0010</t>
   </si>
   <si>
-    <t>OPQA-1688</t>
-  </si>
-  <si>
     <t>DRA0011</t>
   </si>
   <si>
@@ -104,9 +89,6 @@
     <t>DRA0013</t>
   </si>
   <si>
-    <t>OPQA-1689</t>
-  </si>
-  <si>
     <t>forgot PWD</t>
   </si>
   <si>
@@ -119,21 +101,42 @@
     <t>OPQA-TBD</t>
   </si>
   <si>
-    <t xml:space="preserve">Verify that user should  not be allowed to sign-in to DRA when email/password combination is incorrect and error message "Invalid Email/Password. Please try again." should be dispalyed as per  DRA Access - conditional text and error message document.
+    <t>OPQA-4185 ||OPQA-4196</t>
+  </si>
+  <si>
+    <t>Verify that user should not be allowed to access DRA if the STeAM account is not tied to an active subscription with the "DRA_TARGET_DRUG" entitlement (SKU).|| Verify that Error message is displayed to the user, when DRA user who attempts to access DRA without an active DRA entitlement (STeAM SKU)</t>
+  </si>
+  <si>
+    <t>Verify that, accessing of the URL  takes the user to DRA application Landing page || Verify that DRA Landing page, displays application branding and logo || Verify that DRA Landing page, contains feature promotion and iconography in the marketing section || Verify that DRA Landing page, displays link to privacy statement and terms of use. || verify that DRA Landing page, displays the message and email id on the DRA landing page "Having trouble with sign-in? please contact DRA_support@thomsonreuters.com "||Verify that Learn more link is displayed and navigated to the correct page or not</t>
+  </si>
+  <si>
+    <t>OPQA-4176||OPQA-4178||OPQA-4179||OPQA-4182||OPQA-4187||OPQA-4189 </t>
+  </si>
+  <si>
+    <t>OPQA-4233</t>
+  </si>
+  <si>
+    <t>OPQA-4249 ||OPQA-4247 ||OPQA-4238</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Verify that when linking a social with a matching email, if the user click [X] cross mark on the screen then he will be taken back to the DRA Login page. || Verify that text on the modal "Already have an account? .. ||Verify that when linking a social with a matching email, if the user clicks outside the Linking modal on the screen then nothing should happens</t>
+  </si>
+  <si>
+    <t>OPQA-4241||OPQA-4245</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify that user should  not be allowed to sign-in to DRA when email/password combination is incorrect and error message "Invalid Email/Password. Please try again." should be dispalyed as per  DRA Access - conditional text and error message document. ||Verify that user should successfully authenticate to the platform by by supplying correct STeAM credentials (email address + password), on the DRA sign in screen. 
 </t>
   </si>
   <si>
-    <t>OPQA-4185 ||OPQA-4196</t>
-  </si>
-  <si>
-    <t>Verify that user should not be allowed to access DRA if the STeAM account is not tied to an active subscription with the "DRA_TARGET_DRUG" entitlement (SKU).|| Verify that Error message is displayed to the user, when DRA user who attempts to access DRA without an active DRA entitlement (STeAM SKU)</t>
+    <t> OPQA-4180||OPQA-4177</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -147,6 +150,14 @@
       <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -193,10 +204,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -210,8 +222,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
@@ -544,8 +560,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -574,15 +590,15 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>7</v>
+      <c r="B2" s="7" t="s">
+        <v>24</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>6</v>
@@ -591,28 +607,28 @@
     </row>
     <row r="3" spans="1:5" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E3" s="2"/>
     </row>
-    <row r="4" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>26</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>6</v>
@@ -621,28 +637,28 @@
     </row>
     <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>7</v>
+        <v>28</v>
       </c>
       <c r="C5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="2"/>
+    </row>
+    <row r="6" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5" s="2"/>
-    </row>
-    <row r="6" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
-        <v>15</v>
-      </c>
       <c r="B6" s="5" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>6</v>
@@ -651,13 +667,13 @@
     </row>
     <row r="7" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="D7" s="6" t="s">
         <v>6</v>
@@ -666,13 +682,13 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>6</v>
@@ -681,13 +697,13 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="5" t="s">
-        <v>21</v>
-      </c>
       <c r="C9" s="5" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>6</v>
@@ -696,13 +712,13 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>6</v>
@@ -710,7 +726,10 @@
       <c r="E10" s="5"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-4176"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added New Script DRA005
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/DRA.xlsx
+++ b/src/test/resources/xls/DRA.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="2640" windowWidth="13290" windowHeight="3840"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="38">
   <si>
     <t>TCID</t>
   </si>
@@ -143,12 +143,21 @@
   <si>
     <t>Verify that the profile fly-out should contain link to terms of use||Verify that profile fly-out should contain link to privacy statement||Verify that the profile fly-out should contain link to app-specific feedback page (http://thomson-reuters1260211048.drug-research-advisor-target-druggability-feedback.sgizmo.com/s3)||Verify that the profile fly-out should contain link to app-specific help page||Verify that the alternative profile fly-out should contain link to sign out of the platform. User returns to DRA sign-in page.</t>
   </si>
+  <si>
+    <t>DRA005</t>
+  </si>
+  <si>
+    <t>OPQA-4221</t>
+  </si>
+  <si>
+    <t>Verify that error message " Incorrect password. Please try again."should be displayed when user enters incorrect password for existing steam account.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -358,6 +367,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -392,6 +402,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -567,14 +578,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C17" sqref="C16:C17"/>
+      <selection activeCell="A12" sqref="A12:E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.42578125" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="34.42578125" customWidth="1" collapsed="1"/>
@@ -583,7 +594,7 @@
     <col min="5" max="5" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -600,7 +611,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="105">
+    <row r="2" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
@@ -615,7 +626,7 @@
       </c>
       <c r="E2" s="2"/>
     </row>
-    <row r="3" spans="1:5" ht="34.5" customHeight="1">
+    <row r="3" spans="1:5" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>7</v>
       </c>
@@ -630,7 +641,7 @@
       </c>
       <c r="E3" s="2"/>
     </row>
-    <row r="4" spans="1:5" ht="60">
+    <row r="4" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>8</v>
       </c>
@@ -645,7 +656,7 @@
       </c>
       <c r="E4" s="2"/>
     </row>
-    <row r="5" spans="1:5" ht="45">
+    <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>9</v>
       </c>
@@ -660,7 +671,7 @@
       </c>
       <c r="E5" s="2"/>
     </row>
-    <row r="6" spans="1:5" ht="90">
+    <row r="6" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>12</v>
       </c>
@@ -675,7 +686,7 @@
       </c>
       <c r="E6" s="5"/>
     </row>
-    <row r="7" spans="1:5" ht="60">
+    <row r="7" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>13</v>
       </c>
@@ -690,7 +701,7 @@
       </c>
       <c r="E7" s="5"/>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>14</v>
       </c>
@@ -705,7 +716,7 @@
       </c>
       <c r="E8" s="5"/>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>16</v>
       </c>
@@ -720,7 +731,7 @@
       </c>
       <c r="E9" s="5"/>
     </row>
-    <row r="10" spans="1:5" ht="90">
+    <row r="10" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>18</v>
       </c>
@@ -735,7 +746,7 @@
       </c>
       <c r="E10" s="5"/>
     </row>
-    <row r="11" spans="1:5" ht="75">
+    <row r="11" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>30</v>
       </c>
@@ -749,12 +760,28 @@
         <v>6</v>
       </c>
       <c r="E11" s="5"/>
+    </row>
+    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E12" s="5"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-4176"/>
+    <hyperlink ref="B12" r:id="rId2" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-4221"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
New script for OPQA-4190,OPQA-4188
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/DRA.xlsx
+++ b/src/test/resources/xls/DRA.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="2640" windowWidth="13290" windowHeight="3840"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="41">
   <si>
     <t>TCID</t>
   </si>
@@ -152,12 +152,21 @@
   <si>
     <t>Verify that profile fly-out will display profile meta-data||Verify that profile fly-out provides access to the profile modal.||Verify that the profile fly-out should display the following user profile details, if available: a)First name b)Last Name c)Title d)Institution e)Country f)Photo||Verify that by clicking on any of the following fields (when present), will provide access to the profile modal. 1.Name 2.Institution 3. Country 4 .Title 5.Photo || Verify that profile fly-out provides access to the account setting modal</t>
   </si>
+  <si>
+    <t>DRA051</t>
+  </si>
+  <si>
+    <t>OPQA-4188||OPQA-4190</t>
+  </si>
+  <si>
+    <t>Verify that  if the STeAM account is pre-existing and missing a first or last name, the system should populate with a null value in the user's DRA profile.||Verify that a user who has a STeAM account with a missing first name, last name, or both should still be able to log into DRA.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -335,7 +344,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -367,9 +376,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -401,6 +411,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -576,14 +587,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C16" sqref="C15:C16"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C18" sqref="C16:C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.42578125" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="34.42578125" customWidth="1" collapsed="1"/>
@@ -592,7 +603,7 @@
     <col min="5" max="5" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -609,7 +620,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="105">
+    <row r="2" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
@@ -624,7 +635,7 @@
       </c>
       <c r="E2" s="2"/>
     </row>
-    <row r="3" spans="1:5" ht="34.5" customHeight="1">
+    <row r="3" spans="1:5" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>7</v>
       </c>
@@ -639,7 +650,7 @@
       </c>
       <c r="E3" s="2"/>
     </row>
-    <row r="4" spans="1:5" ht="60">
+    <row r="4" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>8</v>
       </c>
@@ -654,7 +665,7 @@
       </c>
       <c r="E4" s="2"/>
     </row>
-    <row r="5" spans="1:5" ht="45">
+    <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>9</v>
       </c>
@@ -669,7 +680,7 @@
       </c>
       <c r="E5" s="2"/>
     </row>
-    <row r="6" spans="1:5" ht="90">
+    <row r="6" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>12</v>
       </c>
@@ -684,7 +695,7 @@
       </c>
       <c r="E6" s="5"/>
     </row>
-    <row r="7" spans="1:5" ht="60">
+    <row r="7" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>13</v>
       </c>
@@ -699,7 +710,7 @@
       </c>
       <c r="E7" s="5"/>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>14</v>
       </c>
@@ -714,7 +725,7 @@
       </c>
       <c r="E8" s="5"/>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>16</v>
       </c>
@@ -729,7 +740,7 @@
       </c>
       <c r="E9" s="5"/>
     </row>
-    <row r="10" spans="1:5" ht="90">
+    <row r="10" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>18</v>
       </c>
@@ -744,7 +755,7 @@
       </c>
       <c r="E10" s="5"/>
     </row>
-    <row r="11" spans="1:5" ht="90">
+    <row r="11" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>30</v>
       </c>
@@ -759,7 +770,7 @@
       </c>
       <c r="E11" s="5"/>
     </row>
-    <row r="12" spans="1:5" ht="30">
+    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>33</v>
       </c>
@@ -773,13 +784,29 @@
         <v>6</v>
       </c>
       <c r="E12" s="5"/>
+    </row>
+    <row r="13" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E13" s="5"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-4176"/>
     <hyperlink ref="B12" r:id="rId2" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-4221"/>
+    <hyperlink ref="B13" r:id="rId3" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-4221"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added New script for OPQA-4224 & OPQA-4223
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/DRA.xlsx
+++ b/src/test/resources/xls/DRA.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="2640" windowWidth="13290" windowHeight="3840"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="44">
   <si>
     <t>TCID</t>
   </si>
@@ -160,6 +160,15 @@
   </si>
   <si>
     <t>Verify that  if the STeAM account is pre-existing and missing a first or last name, the system should populate with a null value in the user's DRA profile.||Verify that a user who has a STeAM account with a missing first name, last name, or both should still be able to log into DRA.</t>
+  </si>
+  <si>
+    <t>DRA006</t>
+  </si>
+  <si>
+    <t>Verify that error message " New password should not match current password" should be displayed when user enters the current password in change password field.|| Verify that error message"New password should not match previous 4 passwords" should be displayed when user enters password in change password field which is matching with the previous 4 passwords.</t>
+  </si>
+  <si>
+    <t>OPQA-4223 || OPQA-4224</t>
   </si>
 </sst>
 </file>
@@ -344,7 +353,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -379,7 +388,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -588,10 +597,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C18" sqref="C16:C18"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -785,28 +794,44 @@
       </c>
       <c r="E12" s="5"/>
     </row>
-    <row r="13" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E13" s="5"/>
+    </row>
+    <row r="14" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B14" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C14" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="D13" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E13" s="5"/>
+      <c r="D14" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E14" s="5"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-4176"/>
-    <hyperlink ref="B12" r:id="rId2" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-4221"/>
-    <hyperlink ref="B13" r:id="rId3" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-4221"/>
+    <hyperlink ref="B14" r:id="rId2" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-4221"/>
+    <hyperlink ref="B12" r:id="rId3" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-4221"/>
+    <hyperlink ref="B13" r:id="rId4" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-4223"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId4"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added New scripts for OPQA-4225 & OPQA-4224
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/DRA.xlsx
+++ b/src/test/resources/xls/DRA.xlsx
@@ -141,12 +141,6 @@
     <t>DRA005</t>
   </si>
   <si>
-    <t>OPQA-4221</t>
-  </si>
-  <si>
-    <t>Verify that error message " Incorrect password. Please try again."should be displayed when user enters incorrect password for existing steam account.</t>
-  </si>
-  <si>
     <t>OPQA-4197||OPQA-4199||OPQA-4215||OPQA-4216||OPQA-4201</t>
   </si>
   <si>
@@ -169,6 +163,12 @@
   </si>
   <si>
     <t>OPQA-4223 || OPQA-4224</t>
+  </si>
+  <si>
+    <t>Verify that error message " Incorrect password. Please try again."should be displayed when user enters incorrect password for existing steam account.|| Verify that when user's account is locked due to 10 invalid authentications of existing password,user becomes locked, the user is signed out</t>
+  </si>
+  <si>
+    <t>OPQA-4221 || OPQA-4225</t>
   </si>
 </sst>
 </file>
@@ -599,8 +599,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -769,25 +769,25 @@
         <v>30</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E11" s="5"/>
     </row>
-    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>33</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>6</v>
@@ -796,13 +796,13 @@
     </row>
     <row r="13" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B13" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B13" s="3" t="s">
-        <v>43</v>
-      </c>
       <c r="C13" s="6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>6</v>
@@ -811,13 +811,13 @@
     </row>
     <row r="14" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14" s="6" t="s">
         <v>38</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>40</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
added jira id to dra052
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/DRA.xlsx
+++ b/src/test/resources/xls/DRA.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="47">
   <si>
     <t>TCID</t>
   </si>
@@ -172,6 +172,12 @@
   </si>
   <si>
     <t>DRA052</t>
+  </si>
+  <si>
+    <t>Verify that, the account link or merge should not be made, if skipping the linking of an existing social account</t>
+  </si>
+  <si>
+    <t>OPQA-4243</t>
   </si>
 </sst>
 </file>
@@ -603,7 +609,7 @@
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -827,15 +833,15 @@
       </c>
       <c r="E14" s="5"/>
     </row>
-    <row r="15" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>44</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>35</v>
+        <v>46</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
IPA new script implementation
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/DRA.xlsx
+++ b/src/test/resources/xls/DRA.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="2640" windowWidth="13290" windowHeight="3840"/>
@@ -105,9 +105,6 @@
   </si>
   <si>
     <t>OPQA-4205||OPQA-4207||OPQA-4208||OPQA-4210||OPQA-4211</t>
-  </si>
-  <si>
-    <t>Verify that the profile fly-out should contain link to terms of use||Verify that profile fly-out should contain link to privacy statement||Verify that the profile fly-out should contain link to app-specific feedback page (http://thomson-reuters1260211048.drug-research-advisor-target-druggability-feedback.sgizmo.com/s3)||Verify that the profile fly-out should contain link to app-specific help page||Verify that the alternative profile fly-out should contain link to sign out of the platform. User returns to DRA sign-in page.</t>
   </si>
   <si>
     <t>DRA005</t>
@@ -206,12 +203,15 @@
   <si>
     <t>From DRA\IPA , Verify that system is able to merge Activated STeAM account and Activated Facebook account and after merge verify STeAM TRUID is change||Verify that If a user signs into DRA \IPA with a STeAM account that has a social account linked, the user should still see their linked social accounts on their account settings page.</t>
   </si>
+  <si>
+    <t>Verify that the profile fly-out should contain link to terms of use||Verify that profile fly-out should contain link to privacy statement||Verify that the profile fly-out should contain link to app-specific feedback page ||Verify that the profile fly-out should contain link to app-specific help page||Verify that the alternative profile fly-out should contain link to sign out of the platform. User returns to sign-in page.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -398,7 +398,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -430,10 +430,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -465,7 +464,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -641,14 +639,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="14.42578125" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="34.42578125" customWidth="1" collapsed="1"/>
@@ -657,7 +655,7 @@
     <col min="5" max="5" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -674,7 +672,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="105">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
@@ -689,22 +687,22 @@
       </c>
       <c r="E2" s="2"/>
     </row>
-    <row r="3" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="60">
       <c r="A3" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E3" s="2"/>
     </row>
-    <row r="4" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="60">
       <c r="A4" s="3" t="s">
         <v>8</v>
       </c>
@@ -719,7 +717,7 @@
       </c>
       <c r="E4" s="2"/>
     </row>
-    <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="45">
       <c r="A5" s="3" t="s">
         <v>9</v>
       </c>
@@ -734,7 +732,7 @@
       </c>
       <c r="E5" s="2"/>
     </row>
-    <row r="6" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="90">
       <c r="A6" s="5" t="s">
         <v>11</v>
       </c>
@@ -749,7 +747,7 @@
       </c>
       <c r="E6" s="5"/>
     </row>
-    <row r="7" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="60">
       <c r="A7" s="5" t="s">
         <v>12</v>
       </c>
@@ -764,7 +762,7 @@
       </c>
       <c r="E7" s="5"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5">
       <c r="A8" s="5" t="s">
         <v>13</v>
       </c>
@@ -779,7 +777,7 @@
       </c>
       <c r="E8" s="5"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5">
       <c r="A9" s="5" t="s">
         <v>15</v>
       </c>
@@ -794,7 +792,7 @@
       </c>
       <c r="E9" s="5"/>
     </row>
-    <row r="10" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="75">
       <c r="A10" s="5" t="s">
         <v>17</v>
       </c>
@@ -802,127 +800,127 @@
         <v>29</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>30</v>
+        <v>55</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>6</v>
       </c>
       <c r="E10" s="5"/>
     </row>
-    <row r="11" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="90">
       <c r="A11" s="5" t="s">
         <v>28</v>
       </c>
       <c r="B11" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="D11" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" s="5"/>
+    </row>
+    <row r="12" spans="1:5" ht="60">
+      <c r="A12" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E12" s="5"/>
+    </row>
+    <row r="13" spans="1:5" ht="75">
+      <c r="A13" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E13" s="5"/>
+    </row>
+    <row r="14" spans="1:5" ht="60">
+      <c r="A14" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D11" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E11" s="5"/>
-    </row>
-    <row r="12" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E12" s="5"/>
-    </row>
-    <row r="13" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E13" s="5"/>
-    </row>
-    <row r="14" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
+      <c r="B14" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="C14" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C14" s="6" t="s">
-        <v>36</v>
-      </c>
       <c r="D14" s="2" t="s">
         <v>6</v>
       </c>
       <c r="E14" s="5"/>
     </row>
-    <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" ht="30">
       <c r="A15" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C15" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="D15" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E15" s="5"/>
+    </row>
+    <row r="16" spans="1:5" ht="30">
+      <c r="A16" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B16" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C15" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E15" s="5"/>
-    </row>
-    <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
+      <c r="C16" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E16" s="5"/>
+    </row>
+    <row r="17" spans="1:5" ht="30">
+      <c r="A17" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="B16" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="C16" s="8" t="s">
+      <c r="B17" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="D16" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E16" s="5"/>
-    </row>
-    <row r="17" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
+      <c r="C17" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E17" s="5"/>
+    </row>
+    <row r="18" spans="1:5" ht="60">
+      <c r="A18" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B18" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="B17" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="C17" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E17" s="5"/>
-    </row>
-    <row r="18" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A18" s="5" t="s">
+      <c r="C18" s="6" t="s">
         <v>54</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="C18" s="6" t="s">
-        <v>55</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
Added IPA scripts and fixed DRA scripts
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/DRA.xlsx
+++ b/src/test/resources/xls/DRA.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="2640" windowWidth="13290" windowHeight="3840"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="59">
   <si>
     <t>TCID</t>
   </si>
@@ -206,12 +206,21 @@
   <si>
     <t>Verify that the profile fly-out should contain link to terms of use||Verify that profile fly-out should contain link to privacy statement||Verify that the profile fly-out should contain link to app-specific feedback page ||Verify that the profile fly-out should contain link to app-specific help page||Verify that the alternative profile fly-out should contain link to sign out of the platform. User returns to sign-in page.</t>
   </si>
+  <si>
+    <t>DRA0016</t>
+  </si>
+  <si>
+    <t>OPQA-4219||OPQA-4218</t>
+  </si>
+  <si>
+    <t>Verify that the accounts setting modal should be accessible to users in non-discoverable state.||Verify that the accounts setting modal should not initiate on-boarding.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -430,6 +439,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -464,6 +474,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -639,14 +650,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.42578125" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="34.42578125" customWidth="1" collapsed="1"/>
@@ -655,7 +666,7 @@
     <col min="5" max="5" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -672,7 +683,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="105">
+    <row r="2" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
@@ -687,7 +698,7 @@
       </c>
       <c r="E2" s="2"/>
     </row>
-    <row r="3" spans="1:5" ht="60">
+    <row r="3" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>7</v>
       </c>
@@ -702,7 +713,7 @@
       </c>
       <c r="E3" s="2"/>
     </row>
-    <row r="4" spans="1:5" ht="60">
+    <row r="4" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>8</v>
       </c>
@@ -717,7 +728,7 @@
       </c>
       <c r="E4" s="2"/>
     </row>
-    <row r="5" spans="1:5" ht="45">
+    <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>9</v>
       </c>
@@ -732,7 +743,7 @@
       </c>
       <c r="E5" s="2"/>
     </row>
-    <row r="6" spans="1:5" ht="90">
+    <row r="6" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>11</v>
       </c>
@@ -747,7 +758,7 @@
       </c>
       <c r="E6" s="5"/>
     </row>
-    <row r="7" spans="1:5" ht="60">
+    <row r="7" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>12</v>
       </c>
@@ -762,7 +773,7 @@
       </c>
       <c r="E7" s="5"/>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>13</v>
       </c>
@@ -777,7 +788,7 @@
       </c>
       <c r="E8" s="5"/>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>15</v>
       </c>
@@ -792,7 +803,7 @@
       </c>
       <c r="E9" s="5"/>
     </row>
-    <row r="10" spans="1:5" ht="75">
+    <row r="10" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>17</v>
       </c>
@@ -807,7 +818,7 @@
       </c>
       <c r="E10" s="5"/>
     </row>
-    <row r="11" spans="1:5" ht="90">
+    <row r="11" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>28</v>
       </c>
@@ -822,7 +833,7 @@
       </c>
       <c r="E11" s="5"/>
     </row>
-    <row r="12" spans="1:5" ht="60">
+    <row r="12" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>30</v>
       </c>
@@ -837,7 +848,7 @@
       </c>
       <c r="E12" s="5"/>
     </row>
-    <row r="13" spans="1:5" ht="75">
+    <row r="13" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>36</v>
       </c>
@@ -852,7 +863,7 @@
       </c>
       <c r="E13" s="5"/>
     </row>
-    <row r="14" spans="1:5" ht="60">
+    <row r="14" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>33</v>
       </c>
@@ -867,7 +878,7 @@
       </c>
       <c r="E14" s="5"/>
     </row>
-    <row r="15" spans="1:5" ht="30">
+    <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>43</v>
       </c>
@@ -882,7 +893,7 @@
       </c>
       <c r="E15" s="5"/>
     </row>
-    <row r="16" spans="1:5" ht="30">
+    <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>50</v>
       </c>
@@ -897,7 +908,7 @@
       </c>
       <c r="E16" s="5"/>
     </row>
-    <row r="17" spans="1:5" ht="30">
+    <row r="17" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>51</v>
       </c>
@@ -912,7 +923,7 @@
       </c>
       <c r="E17" s="5"/>
     </row>
-    <row r="18" spans="1:5" ht="60">
+    <row r="18" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>53</v>
       </c>
@@ -926,6 +937,21 @@
         <v>6</v>
       </c>
       <c r="E18" s="5"/>
+    </row>
+    <row r="19" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E19" s="5"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Added New script for DRA
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/DRA.xlsx
+++ b/src/test/resources/xls/DRA.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="63">
   <si>
     <t>TCID</t>
   </si>
@@ -218,12 +218,21 @@
   <si>
     <t>Verify that user should not be allowed to sign-in to DRA \IPA when user account is locked ||Verify that user should not be allowed to sign-in to DRA \IPA when user account is evicted/Suspended .</t>
   </si>
+  <si>
+    <t>DRA0017</t>
+  </si>
+  <si>
+    <t>OPQA-4525||OPQA-4526||OPQA-4527</t>
+  </si>
+  <si>
+    <t>Verify that the STeAM Step Up Auth Modal should be presented to the user without a pre-populated email address when user has a valid Neon session token and is navigating within the same browser window.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -251,6 +260,13 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -301,7 +317,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -320,6 +336,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -654,10 +673,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -956,6 +975,21 @@
       </c>
       <c r="E19" s="5"/>
     </row>
+    <row r="20" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E20" s="5"/>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-4176"/>

</xml_diff>

<commit_message>
New script in DRA
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/DRA.xlsx
+++ b/src/test/resources/xls/DRA.xlsx
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="125725" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="66">
   <si>
     <t>TCID</t>
   </si>
@@ -226,6 +226,15 @@
   </si>
   <si>
     <t>Verify that the STeAM Step Up Auth Modal should be presented to the user without a pre-populated email address when user has a valid Neon session token and is navigating within the same browser window.</t>
+  </si>
+  <si>
+    <t>DRA007</t>
+  </si>
+  <si>
+    <t>OPQA-4531||OPQA-4533</t>
+  </si>
+  <si>
+    <t>Verify that the new STeAM step up authentication modal should include a link to initiate the EndNote supported forgot password flow. || Verify that the "Sign in to Target Druggability" modal should match with wireframe</t>
   </si>
 </sst>
 </file>
@@ -673,10 +682,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="A21" sqref="A21:E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -990,6 +999,21 @@
       </c>
       <c r="E20" s="5"/>
     </row>
+    <row r="21" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E21" s="5"/>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" display="http://jira.bjz.apac.ime.reuters.com/browse/OPQA-4176"/>

</xml_diff>

<commit_message>
Added Forgot password Scripts in DRA and IPA application.
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/DRA.xlsx
+++ b/src/test/resources/xls/DRA.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2640" windowWidth="13290" windowHeight="3840"/>
+    <workbookView xWindow="0" yWindow="2640" windowWidth="13296" windowHeight="3840"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725" concurrentCalc="0"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="69">
   <si>
     <t>TCID</t>
   </si>
@@ -236,12 +236,30 @@
   <si>
     <t>Verify that the new STeAM step up authentication modal should include a link to initiate the EndNote supported forgot password flow. || Verify that the "Sign in to Target Druggability" modal should match with wireframe</t>
   </si>
+  <si>
+    <t>DRA100</t>
+  </si>
+  <si>
+    <t>OPQA-1934||
+OPQA-1935&amp;OPQA-3687||
+OPQA-4230||OPQA-4229||
+OPQA-4231||OPQA-4232||
+OPQA-4636||OPQA-4261||
+OPQA-4244||OPQA-4264||
+OPQA-4265||OPQA-4237||
+OPQA-4239||OPQA-4240||
+OPQA-4246||OPQA-4248||
+OPQA-4252</t>
+  </si>
+  <si>
+    <t>Verify that Forgot your password? Link is clickable on NEON Landing page and End note landing page||Verify that the system is navigating to Forgot Password page or not, after clicking on Forgot your password? Link&amp;Verify that,the system should support a ENW password reset workflow with the following configurations||Verify that system should not inform user that entered email is not found.||Verify that user should be able to enter email address in Forgot password page.||Verify that  forget password service should send a forgot password email when the email entered is registered in the system||Verify that the platform password reset service should send a platform forget password email with branding that corresponds with the originating application as per wireframe||Verify that When the password reset token in the email is valid, upon clicking the password reset link in the the platform forget password email, the user shall be taken to the External Password Reset Page||Verify that External Password Reset Page should have a new password field where the user enters their new password.||Verify that when reset Password Token already used user should be taken to sign in screen||Verify that upon successful submission of a password change, The user should receive a password change confirmation email to the user's primary email address with branding that corresponds with the application that the user completed the password change||Verify that the password change confirmation email should reference the fact that credentials are shared across all products.||Verify that when the password reset token in the email is expired or already used, upon clicking the password reset link in the the platform forget password email, the user should be taken to the External Invalid Password Reset Token Page.||Verify that the email address on the External Invalid Password Reset Token Page should be pre-populated with the email address that matches the email that the forgot password email was sent.||Verify that user who clicks the submit button on the the External Invalid Password Reset Token page, should be taken to the target application sign in page.||Verify that when Email address is known from password reset token,error message 'The email address is prepopulated.' should be displayed and email address field should be editable||Verify that when Email address is not known from password reset token,email address field should be blank and user should be able to enter any email address||Verify that error message Please enter a valid email address.should be displayed in red color when user enters email address in wrong format</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -470,7 +488,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -505,7 +522,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -681,23 +697,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21:E21"/>
+      <selection activeCell="A22" sqref="A22:E22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="34.42578125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="86.28515625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="25.28515625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="14.44140625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="34.44140625" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="86.33203125" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="25.33203125" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="7.33203125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -714,7 +730,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="100.8">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
@@ -729,7 +745,7 @@
       </c>
       <c r="E2" s="2"/>
     </row>
-    <row r="3" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="57.6">
       <c r="A3" s="3" t="s">
         <v>7</v>
       </c>
@@ -744,7 +760,7 @@
       </c>
       <c r="E3" s="2"/>
     </row>
-    <row r="4" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="57.6">
       <c r="A4" s="3" t="s">
         <v>8</v>
       </c>
@@ -759,7 +775,7 @@
       </c>
       <c r="E4" s="2"/>
     </row>
-    <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="28.8">
       <c r="A5" s="3" t="s">
         <v>9</v>
       </c>
@@ -774,7 +790,7 @@
       </c>
       <c r="E5" s="2"/>
     </row>
-    <row r="6" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="86.4">
       <c r="A6" s="5" t="s">
         <v>11</v>
       </c>
@@ -789,7 +805,7 @@
       </c>
       <c r="E6" s="5"/>
     </row>
-    <row r="7" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="57.6">
       <c r="A7" s="5" t="s">
         <v>12</v>
       </c>
@@ -804,7 +820,7 @@
       </c>
       <c r="E7" s="5"/>
     </row>
-    <row r="8" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="28.8">
       <c r="A8" s="5" t="s">
         <v>13</v>
       </c>
@@ -819,7 +835,7 @@
       </c>
       <c r="E8" s="5"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5">
       <c r="A9" s="5" t="s">
         <v>14</v>
       </c>
@@ -834,7 +850,7 @@
       </c>
       <c r="E9" s="5"/>
     </row>
-    <row r="10" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="72">
       <c r="A10" s="5" t="s">
         <v>15</v>
       </c>
@@ -849,7 +865,7 @@
       </c>
       <c r="E10" s="5"/>
     </row>
-    <row r="11" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="86.4">
       <c r="A11" s="5" t="s">
         <v>25</v>
       </c>
@@ -864,7 +880,7 @@
       </c>
       <c r="E11" s="5"/>
     </row>
-    <row r="12" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="43.2">
       <c r="A12" s="5" t="s">
         <v>27</v>
       </c>
@@ -879,7 +895,7 @@
       </c>
       <c r="E12" s="5"/>
     </row>
-    <row r="13" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="57.6">
       <c r="A13" s="5" t="s">
         <v>33</v>
       </c>
@@ -894,7 +910,7 @@
       </c>
       <c r="E13" s="5"/>
     </row>
-    <row r="14" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="43.2">
       <c r="A14" s="5" t="s">
         <v>30</v>
       </c>
@@ -909,7 +925,7 @@
       </c>
       <c r="E14" s="5"/>
     </row>
-    <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" ht="28.8">
       <c r="A15" s="5" t="s">
         <v>40</v>
       </c>
@@ -924,7 +940,7 @@
       </c>
       <c r="E15" s="5"/>
     </row>
-    <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" ht="28.8">
       <c r="A16" s="2" t="s">
         <v>47</v>
       </c>
@@ -939,7 +955,7 @@
       </c>
       <c r="E16" s="5"/>
     </row>
-    <row r="17" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" ht="28.8">
       <c r="A17" s="5" t="s">
         <v>48</v>
       </c>
@@ -954,7 +970,7 @@
       </c>
       <c r="E17" s="5"/>
     </row>
-    <row r="18" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" ht="57.6">
       <c r="A18" s="5" t="s">
         <v>50</v>
       </c>
@@ -969,7 +985,7 @@
       </c>
       <c r="E18" s="5"/>
     </row>
-    <row r="19" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" ht="28.8">
       <c r="A19" s="5" t="s">
         <v>53</v>
       </c>
@@ -984,7 +1000,7 @@
       </c>
       <c r="E19" s="5"/>
     </row>
-    <row r="20" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" ht="43.2">
       <c r="A20" s="5" t="s">
         <v>60</v>
       </c>
@@ -999,7 +1015,7 @@
       </c>
       <c r="E20" s="5"/>
     </row>
-    <row r="21" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" ht="43.2">
       <c r="A21" s="5" t="s">
         <v>63</v>
       </c>
@@ -1013,6 +1029,21 @@
         <v>6</v>
       </c>
       <c r="E21" s="5"/>
+    </row>
+    <row r="22" spans="1:5" ht="172.8">
+      <c r="A22" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E22" s="5"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Added New scripts for DRA Stepup Auth modal
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/DRA.xlsx
+++ b/src/test/resources/xls/DRA.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2640" windowWidth="13296" windowHeight="3840"/>
+    <workbookView xWindow="0" yWindow="2640" windowWidth="13290" windowHeight="3840"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="125725" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="72">
   <si>
     <t>TCID</t>
   </si>
@@ -231,12 +231,6 @@
     <t>DRA007</t>
   </si>
   <si>
-    <t>OPQA-4531||OPQA-4533</t>
-  </si>
-  <si>
-    <t>Verify that the new STeAM step up authentication modal should include a link to initiate the EndNote supported forgot password flow. || Verify that the "Sign in to Target Druggability" modal should match with wireframe</t>
-  </si>
-  <si>
     <t>DRA100</t>
   </si>
   <si>
@@ -254,12 +248,27 @@
   <si>
     <t>Verify that Forgot your password? Link is clickable on NEON Landing page and End note landing page||Verify that the system is navigating to Forgot Password page or not, after clicking on Forgot your password? Link&amp;Verify that,the system should support a ENW password reset workflow with the following configurations||Verify that system should not inform user that entered email is not found.||Verify that user should be able to enter email address in Forgot password page.||Verify that  forget password service should send a forgot password email when the email entered is registered in the system||Verify that the platform password reset service should send a platform forget password email with branding that corresponds with the originating application as per wireframe||Verify that When the password reset token in the email is valid, upon clicking the password reset link in the the platform forget password email, the user shall be taken to the External Password Reset Page||Verify that External Password Reset Page should have a new password field where the user enters their new password.||Verify that when reset Password Token already used user should be taken to sign in screen||Verify that upon successful submission of a password change, The user should receive a password change confirmation email to the user's primary email address with branding that corresponds with the application that the user completed the password change||Verify that the password change confirmation email should reference the fact that credentials are shared across all products.||Verify that when the password reset token in the email is expired or already used, upon clicking the password reset link in the the platform forget password email, the user should be taken to the External Invalid Password Reset Token Page.||Verify that the email address on the External Invalid Password Reset Token Page should be pre-populated with the email address that matches the email that the forgot password email was sent.||Verify that user who clicks the submit button on the the External Invalid Password Reset Token page, should be taken to the target application sign in page.||Verify that when Email address is known from password reset token,error message 'The email address is prepopulated.' should be displayed and email address field should be editable||Verify that when Email address is not known from password reset token,email address field should be blank and user should be able to enter any email address||Verify that error message Please enter a valid email address.should be displayed in red color when user enters email address in wrong format</t>
   </si>
+  <si>
+    <t>OPQA-4531||OPQA-4533||OPQA-4547||OPQA-4550</t>
+  </si>
+  <si>
+    <t>Verify that the new STeAM step up authentication modal should include a link to initiate the EndNote supported forgot password flow. || Verify that the "Sign in to Target Druggability" modal should match with wireframe || Verify that the target application product overview page should be opened in a separate browser window when User clicks "Learn more" in any of the Step up related messages/modals.||Verify that the DRA\IPA application overview page should be opened in a separate browser window when user has a valid session token on the Neon platform</t>
+  </si>
+  <si>
+    <t>DRA008</t>
+  </si>
+  <si>
+    <t>OPQA-4543 || OPQA-4544</t>
+  </si>
+  <si>
+    <t>Verify that the user should be seamlessly signed into the the target application (DRA/IPA) when target application requires in session steam account authentication. || Verify that the user should be seamlessly signed into the the target application (DRA/IPA) when user has a valid session token on the Neon platform and is navigating within the same browser window.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -344,7 +353,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -363,6 +372,13 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -405,9 +421,6 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -488,6 +501,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -522,6 +536,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -697,23 +712,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E22"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22:E22"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="34.44140625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="86.33203125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="25.33203125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="7.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="14.42578125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="34.42578125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="86.28515625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="25.28515625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -730,7 +745,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="100.8">
+    <row r="2" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
@@ -745,7 +760,7 @@
       </c>
       <c r="E2" s="2"/>
     </row>
-    <row r="3" spans="1:5" ht="57.6">
+    <row r="3" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>7</v>
       </c>
@@ -760,7 +775,7 @@
       </c>
       <c r="E3" s="2"/>
     </row>
-    <row r="4" spans="1:5" ht="57.6">
+    <row r="4" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>8</v>
       </c>
@@ -775,7 +790,7 @@
       </c>
       <c r="E4" s="2"/>
     </row>
-    <row r="5" spans="1:5" ht="28.8">
+    <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>9</v>
       </c>
@@ -790,7 +805,7 @@
       </c>
       <c r="E5" s="2"/>
     </row>
-    <row r="6" spans="1:5" ht="86.4">
+    <row r="6" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>11</v>
       </c>
@@ -805,7 +820,7 @@
       </c>
       <c r="E6" s="5"/>
     </row>
-    <row r="7" spans="1:5" ht="57.6">
+    <row r="7" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>12</v>
       </c>
@@ -820,7 +835,7 @@
       </c>
       <c r="E7" s="5"/>
     </row>
-    <row r="8" spans="1:5" ht="28.8">
+    <row r="8" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>13</v>
       </c>
@@ -835,7 +850,7 @@
       </c>
       <c r="E8" s="5"/>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>14</v>
       </c>
@@ -850,7 +865,7 @@
       </c>
       <c r="E9" s="5"/>
     </row>
-    <row r="10" spans="1:5" ht="72">
+    <row r="10" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>15</v>
       </c>
@@ -865,7 +880,7 @@
       </c>
       <c r="E10" s="5"/>
     </row>
-    <row r="11" spans="1:5" ht="86.4">
+    <row r="11" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>25</v>
       </c>
@@ -880,7 +895,7 @@
       </c>
       <c r="E11" s="5"/>
     </row>
-    <row r="12" spans="1:5" ht="43.2">
+    <row r="12" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>27</v>
       </c>
@@ -895,7 +910,7 @@
       </c>
       <c r="E12" s="5"/>
     </row>
-    <row r="13" spans="1:5" ht="57.6">
+    <row r="13" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
         <v>33</v>
       </c>
@@ -910,7 +925,7 @@
       </c>
       <c r="E13" s="5"/>
     </row>
-    <row r="14" spans="1:5" ht="43.2">
+    <row r="14" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>30</v>
       </c>
@@ -925,7 +940,7 @@
       </c>
       <c r="E14" s="5"/>
     </row>
-    <row r="15" spans="1:5" ht="28.8">
+    <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
         <v>40</v>
       </c>
@@ -940,7 +955,7 @@
       </c>
       <c r="E15" s="5"/>
     </row>
-    <row r="16" spans="1:5" ht="28.8">
+    <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>47</v>
       </c>
@@ -955,7 +970,7 @@
       </c>
       <c r="E16" s="5"/>
     </row>
-    <row r="17" spans="1:5" ht="28.8">
+    <row r="17" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>48</v>
       </c>
@@ -970,7 +985,7 @@
       </c>
       <c r="E17" s="5"/>
     </row>
-    <row r="18" spans="1:5" ht="57.6">
+    <row r="18" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>50</v>
       </c>
@@ -985,7 +1000,7 @@
       </c>
       <c r="E18" s="5"/>
     </row>
-    <row r="19" spans="1:5" ht="28.8">
+    <row r="19" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>53</v>
       </c>
@@ -1000,7 +1015,7 @@
       </c>
       <c r="E19" s="5"/>
     </row>
-    <row r="20" spans="1:5" ht="43.2">
+    <row r="20" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>60</v>
       </c>
@@ -1015,35 +1030,50 @@
       </c>
       <c r="E20" s="5"/>
     </row>
-    <row r="21" spans="1:5" ht="43.2">
-      <c r="A21" s="5" t="s">
+    <row r="21" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A21" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="B21" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="C21" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="D21" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E21" s="10"/>
+    </row>
+    <row r="22" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A22" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="B22" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="C22" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="D22" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E22" s="10"/>
+    </row>
+    <row r="23" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A23" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="C21" s="9" t="s">
+      <c r="B23" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="D21" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E21" s="5"/>
-    </row>
-    <row r="22" spans="1:5" ht="172.8">
-      <c r="A22" s="5" t="s">
+      <c r="C23" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="B22" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="C22" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E22" s="5"/>
+      <c r="D23" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E23" s="5"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>